<commit_message>
update in vitro scripts and in vivo colonization analysis
</commit_message>
<xml_diff>
--- a/LoperamideStrainInfo.xlsx
+++ b/LoperamideStrainInfo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rstevick/Documents/Research/LoperamideMicrobiota/Repo_LoperamideZebrafishDysbiosis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF0B191C-953D-B947-B611-AAC599D496BC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA4B2E20-A4D8-1F44-87D2-A96ADED2D727}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8920" yWindow="5320" windowWidth="34760" windowHeight="18040" xr2:uid="{2F21C9AE-F5C9-EC4D-85E4-2E54FE82CACF}"/>
   </bookViews>
@@ -156,9 +156,6 @@
     <t>Strain</t>
   </si>
   <si>
-    <t>W6t</t>
-  </si>
-  <si>
     <t>CodeName</t>
   </si>
   <si>
@@ -178,6 +175,9 @@
   </si>
   <si>
     <t>Aeromonas veronii</t>
+  </si>
+  <si>
+    <t>W6</t>
   </si>
 </sst>
 </file>
@@ -623,7 +623,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -651,10 +651,10 @@
         <v>15</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H1" s="1"/>
     </row>
@@ -679,7 +679,7 @@
         <v>S1. *Pseudomonas mossellii*</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -687,7 +687,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>14</v>
@@ -703,7 +703,7 @@
         <v>S2. *Variovorax gossypii*</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -727,7 +727,7 @@
         <v>S3. *Pseudomonas nitroreducens*</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -751,7 +751,7 @@
         <v>S4. *Achromobacter marplatensis*</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -775,7 +775,7 @@
         <v>S5. *Stenotrophomas maltophilia*</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -799,7 +799,7 @@
         <v>S6. *Aeromonas caviae*</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -816,14 +816,14 @@
         <v>30</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F8" s="6" t="str">
         <f t="shared" si="0"/>
         <v>S7. *Aeromonas veronii*</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -847,7 +847,7 @@
         <v>S8. *Rhizobium sp.*</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -864,19 +864,19 @@
         <v>32</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F10" s="6" t="str">
         <f t="shared" si="0"/>
         <v>S9. *Ochrobactrum tritici*</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>12</v>
@@ -895,7 +895,7 @@
         <v>S10. *Flavobacterium johnsoniae*</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H11" s="5"/>
     </row>

</xml_diff>